<commit_message>
Jun 10, 2024, 11:53 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/Spell List.xlsx
+++ b/Main/static/CSVs/Spell List.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AD933F-8EFD-4CE2-AC79-EAEA1EC1EBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD9AA99-BE37-439C-AD1F-1DC198CB998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4E9445F3-B443-4A9F-82FC-549874AD4368}"/>
   </bookViews>
   <sheets>
     <sheet name="Spells" sheetId="1" r:id="rId1"/>
-    <sheet name="Lists" sheetId="2" r:id="rId2"/>
-    <sheet name="Spells_no_header" sheetId="3" r:id="rId3"/>
+    <sheet name="SPELL CHANGES" sheetId="4" r:id="rId2"/>
+    <sheet name="Lists" sheetId="2" r:id="rId3"/>
+    <sheet name="Spells_no_header" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2613" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2614" uniqueCount="434">
   <si>
     <t>Acid Splash</t>
   </si>
@@ -1326,6 +1327,9 @@
   </si>
   <si>
     <t>Until triggered</t>
+  </si>
+  <si>
+    <t>Hunter's Mark is now a Cantrip and does not require concentration. Rangers also learn Druidcraft.</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1814,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D16AED1-C2D5-4E4E-BB14-95BEFB4B6974}">
   <dimension ref="A1:T320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L164" sqref="L164"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7712,7 +7718,7 @@
         <v>0</v>
       </c>
       <c r="Q95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R95">
         <v>0</v>
@@ -11948,7 +11954,7 @@
         <v>178</v>
       </c>
       <c r="C164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D164" t="s">
         <v>47</v>
@@ -11975,7 +11981,7 @@
         <v>405</v>
       </c>
       <c r="L164">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M164">
         <v>0</v>
@@ -21683,6 +21689,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E3DEF3B-B5D8-4F41-8F51-A446718EE0A6}">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E9715C-0B9B-43B7-9CF2-094EE36F83D3}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -21970,7 +21996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20437B86-1D70-45B5-9840-1C592BC4A7B2}">
   <dimension ref="A1:N318"/>
   <sheetViews>

</xml_diff>

<commit_message>
Jun 11, 2024, 2:50 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/Spell List.xlsx
+++ b/Main/static/CSVs/Spell List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD9AA99-BE37-439C-AD1F-1DC198CB998D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A68BD8-68DF-4145-B186-55365415EF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4E9445F3-B443-4A9F-82FC-549874AD4368}"/>
   </bookViews>
@@ -1815,7 +1815,7 @@
   <dimension ref="A1:T320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L164" sqref="L164"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Jun 16, 2024, 6:54 PM
</commit_message>
<xml_diff>
--- a/Main/static/CSVs/Spell List.xlsx
+++ b/Main/static/CSVs/Spell List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\CS50-FinalProject\Main\static\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A68BD8-68DF-4145-B186-55365415EF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4752304-744C-436E-BDD5-647EBA1F0C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4E9445F3-B443-4A9F-82FC-549874AD4368}"/>
   </bookViews>
@@ -1815,7 +1815,7 @@
   <dimension ref="A1:T320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>